<commit_message>
Product Backlog with highlights
</commit_message>
<xml_diff>
--- a/ProductBacklogSprint3.xlsx
+++ b/ProductBacklogSprint3.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/schaperg/Documents/PrivateDrive/Courses/__Spring22/CSCI234/Project/SandwichTruck/CurrentVersion/Sprint3/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/colinconway/Courses/Software_engineering/sandwichTruckProj./"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{466C6201-A75A-0A45-BAB9-00F618BD5C8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{863F5AF6-5E86-1F43-BAFD-2C441AF8EBB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -428,7 +428,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -515,8 +515,29 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -529,8 +550,23 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -586,12 +622,30 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -643,9 +697,24 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="1" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="5" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="5">
+    <cellStyle name="Bad" xfId="3" builtinId="27"/>
+    <cellStyle name="Good" xfId="2" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Neutral" xfId="4" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -963,8 +1032,8 @@
   </sheetPr>
   <dimension ref="B1:H52"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A14" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1043,7 +1112,7 @@
       <c r="E8" s="15">
         <v>5</v>
       </c>
-      <c r="F8" s="15">
+      <c r="F8" s="21">
         <v>1</v>
       </c>
       <c r="G8" s="15" t="s">
@@ -1066,7 +1135,7 @@
       <c r="E9" s="15">
         <v>5</v>
       </c>
-      <c r="F9" s="15">
+      <c r="F9" s="21">
         <v>1</v>
       </c>
       <c r="G9" s="15" t="s">
@@ -1089,7 +1158,7 @@
       <c r="E10" s="15">
         <v>5</v>
       </c>
-      <c r="F10" s="15">
+      <c r="F10" s="21">
         <v>1</v>
       </c>
       <c r="G10" s="15" t="s">
@@ -1112,7 +1181,7 @@
       <c r="E11" s="15">
         <v>4</v>
       </c>
-      <c r="F11" s="15">
+      <c r="F11" s="22">
         <v>2</v>
       </c>
       <c r="G11" s="15" t="s">
@@ -1135,7 +1204,7 @@
       <c r="E12" s="15">
         <v>4</v>
       </c>
-      <c r="F12" s="15">
+      <c r="F12" s="22">
         <v>2</v>
       </c>
       <c r="G12" s="15" t="s">
@@ -1158,7 +1227,7 @@
       <c r="E13" s="15">
         <v>3</v>
       </c>
-      <c r="F13" s="15">
+      <c r="F13" s="22">
         <v>2</v>
       </c>
       <c r="G13" s="15" t="s">
@@ -1181,7 +1250,7 @@
       <c r="E14" s="15">
         <v>2</v>
       </c>
-      <c r="F14" s="15">
+      <c r="F14" s="20">
         <v>3</v>
       </c>
       <c r="G14" s="15" t="s">
@@ -1204,7 +1273,7 @@
       <c r="E15" s="15">
         <v>2</v>
       </c>
-      <c r="F15" s="15">
+      <c r="F15" s="19">
         <v>3</v>
       </c>
       <c r="G15" s="15" t="s">
@@ -1269,7 +1338,7 @@
       <c r="E18" s="15">
         <v>1</v>
       </c>
-      <c r="F18" s="15">
+      <c r="F18" s="19">
         <v>3</v>
       </c>
       <c r="G18" s="15" t="s">
@@ -1355,7 +1424,7 @@
       <c r="E22" s="15">
         <v>4</v>
       </c>
-      <c r="F22" s="15">
+      <c r="F22" s="22">
         <v>2</v>
       </c>
       <c r="G22" s="15" t="s">
@@ -1378,7 +1447,7 @@
       <c r="E23" s="15">
         <v>4</v>
       </c>
-      <c r="F23" s="15">
+      <c r="F23" s="22">
         <v>2</v>
       </c>
       <c r="G23" s="15" t="s">
@@ -1401,7 +1470,7 @@
       <c r="E24" s="15">
         <v>5</v>
       </c>
-      <c r="F24" s="15">
+      <c r="F24" s="19">
         <v>3</v>
       </c>
       <c r="G24" s="15" t="s">
@@ -1445,7 +1514,7 @@
       <c r="E26" s="15">
         <v>5</v>
       </c>
-      <c r="F26" s="15">
+      <c r="F26" s="19">
         <v>3</v>
       </c>
       <c r="G26" s="15" t="s">

</xml_diff>